<commit_message>
finished upgraded new form survey
</commit_message>
<xml_diff>
--- a/files/242_ds_mon_hoc.xlsx
+++ b/files/242_ds_mon_hoc.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\tu_hoc\form_api_python\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\googleform_api_python\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F59142-F1BB-496D-A420-ACA982BFE0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A829C1E2-D06F-48FE-A0F5-3DBCE2908F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$V$493</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$V$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3882,35 +3882,35 @@
   </sheetPr>
   <dimension ref="A1:V493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T11" sqref="T11"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="3" customWidth="1"/>
-    <col min="10" max="11" width="14.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="33.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="4" customWidth="1"/>
-    <col min="14" max="14" width="21.28515625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="14.5546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="33.88671875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="21.33203125" style="1" customWidth="1"/>
     <col min="15" max="15" width="35" style="1" customWidth="1"/>
-    <col min="16" max="17" width="9.28515625" style="5" customWidth="1"/>
+    <col min="16" max="17" width="9.33203125" style="5" customWidth="1"/>
     <col min="18" max="18" width="10" style="4" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" style="4" customWidth="1"/>
-    <col min="20" max="20" width="23.5703125" style="4" customWidth="1"/>
-    <col min="21" max="21" width="7.5703125" style="6" customWidth="1"/>
+    <col min="19" max="19" width="17.88671875" style="4" customWidth="1"/>
+    <col min="20" max="20" width="23.5546875" style="4" customWidth="1"/>
+    <col min="21" max="21" width="7.5546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>153</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>153</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>153</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>829</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>834</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>144</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>267</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>623</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>680</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>88</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>88</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>88</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>252</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>252</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>252</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>252</v>
       </c>
@@ -5063,7 +5063,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>252</v>
       </c>
@@ -5131,7 +5131,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>153</v>
       </c>
@@ -5199,7 +5199,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>600</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>275</v>
       </c>
@@ -5335,7 +5335,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>275</v>
       </c>
@@ -5403,7 +5403,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>576</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>588</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>653</v>
       </c>
@@ -5607,7 +5607,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>653</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>924</v>
       </c>
@@ -5743,7 +5743,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>147</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>269</v>
       </c>
@@ -5879,7 +5879,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>269</v>
       </c>
@@ -5947,7 +5947,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>857</v>
       </c>
@@ -6015,7 +6015,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>765</v>
       </c>
@@ -6083,7 +6083,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>417</v>
       </c>
@@ -6151,7 +6151,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>417</v>
       </c>
@@ -6219,7 +6219,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>417</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>417</v>
       </c>
@@ -6355,7 +6355,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>43</v>
       </c>
@@ -6423,7 +6423,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
@@ -6491,7 +6491,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -6559,7 +6559,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>43</v>
       </c>
@@ -6627,7 +6627,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>493</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
@@ -6763,7 +6763,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
@@ -6831,7 +6831,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -6899,7 +6899,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>71</v>
       </c>
@@ -6967,7 +6967,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>179</v>
       </c>
@@ -7035,7 +7035,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>179</v>
       </c>
@@ -7103,7 +7103,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>71</v>
       </c>
@@ -7171,7 +7171,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>179</v>
       </c>
@@ -7239,7 +7239,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>179</v>
       </c>
@@ -7307,7 +7307,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>337</v>
       </c>
@@ -7375,7 +7375,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>513</v>
       </c>
@@ -7443,7 +7443,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>581</v>
       </c>
@@ -7511,7 +7511,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>838</v>
       </c>
@@ -7579,7 +7579,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>71</v>
       </c>
@@ -7647,7 +7647,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>71</v>
       </c>
@@ -7715,7 +7715,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>71</v>
       </c>
@@ -7783,7 +7783,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>71</v>
       </c>
@@ -7851,7 +7851,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>71</v>
       </c>
@@ -7919,7 +7919,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>71</v>
       </c>
@@ -7987,7 +7987,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>697</v>
       </c>
@@ -8055,7 +8055,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>441</v>
       </c>
@@ -8123,7 +8123,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>712</v>
       </c>
@@ -8191,7 +8191,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>903</v>
       </c>
@@ -8259,7 +8259,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>179</v>
       </c>
@@ -8327,7 +8327,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>179</v>
       </c>
@@ -8395,7 +8395,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>179</v>
       </c>
@@ -8463,7 +8463,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>179</v>
       </c>
@@ -8531,7 +8531,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>310</v>
       </c>
@@ -8599,7 +8599,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>402</v>
       </c>
@@ -8667,7 +8667,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>552</v>
       </c>
@@ -8735,7 +8735,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>614</v>
       </c>
@@ -8803,7 +8803,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>915</v>
       </c>
@@ -8871,7 +8871,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>340</v>
       </c>
@@ -8939,7 +8939,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>343</v>
       </c>
@@ -9007,7 +9007,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>721</v>
       </c>
@@ -9075,7 +9075,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>779</v>
       </c>
@@ -9143,7 +9143,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>188</v>
       </c>
@@ -9211,7 +9211,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>188</v>
       </c>
@@ -9279,7 +9279,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>82</v>
       </c>
@@ -9347,7 +9347,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>188</v>
       </c>
@@ -9415,7 +9415,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>82</v>
       </c>
@@ -9483,7 +9483,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>188</v>
       </c>
@@ -9551,7 +9551,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>188</v>
       </c>
@@ -9619,7 +9619,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>505</v>
       </c>
@@ -9687,7 +9687,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>508</v>
       </c>
@@ -9755,7 +9755,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>223</v>
       </c>
@@ -9823,7 +9823,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>805</v>
       </c>
@@ -9891,7 +9891,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>217</v>
       </c>
@@ -9959,7 +9959,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>49</v>
       </c>
@@ -10027,7 +10027,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>126</v>
       </c>
@@ -10095,7 +10095,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>126</v>
       </c>
@@ -10163,7 +10163,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>49</v>
       </c>
@@ -10231,7 +10231,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>350</v>
       </c>
@@ -10299,7 +10299,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>297</v>
       </c>
@@ -10367,7 +10367,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>350</v>
       </c>
@@ -10435,7 +10435,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>726</v>
       </c>
@@ -10503,7 +10503,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>144</v>
       </c>
@@ -10571,7 +10571,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>685</v>
       </c>
@@ -10639,7 +10639,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>685</v>
       </c>
@@ -10707,7 +10707,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>129</v>
       </c>
@@ -10775,7 +10775,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>129</v>
       </c>
@@ -10843,7 +10843,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>129</v>
       </c>
@@ -10911,7 +10911,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>620</v>
       </c>
@@ -10979,7 +10979,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>20</v>
       </c>
@@ -11047,7 +11047,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>58</v>
       </c>
@@ -11115,7 +11115,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>33</v>
       </c>
@@ -11183,7 +11183,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>374</v>
       </c>
@@ -11251,7 +11251,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>33</v>
       </c>
@@ -11319,7 +11319,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>120</v>
       </c>
@@ -11387,7 +11387,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>374</v>
       </c>
@@ -11455,7 +11455,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>374</v>
       </c>
@@ -11523,7 +11523,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="113" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>560</v>
       </c>
@@ -11591,7 +11591,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="114" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>91</v>
       </c>
@@ -11659,7 +11659,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>91</v>
       </c>
@@ -11727,7 +11727,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>88</v>
       </c>
@@ -11795,7 +11795,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="117" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>88</v>
       </c>
@@ -11863,7 +11863,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>86</v>
       </c>
@@ -11931,7 +11931,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>86</v>
       </c>
@@ -11999,7 +11999,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>86</v>
       </c>
@@ -12067,7 +12067,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>642</v>
       </c>
@@ -12135,7 +12135,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>651</v>
       </c>
@@ -12203,7 +12203,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>651</v>
       </c>
@@ -12271,7 +12271,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>726</v>
       </c>
@@ -12339,7 +12339,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>241</v>
       </c>
@@ -12407,7 +12407,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="126" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>123</v>
       </c>
@@ -12475,7 +12475,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="127" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>123</v>
       </c>
@@ -12543,7 +12543,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="128" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>368</v>
       </c>
@@ -12611,7 +12611,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="129" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>123</v>
       </c>
@@ -12679,7 +12679,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="130" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>123</v>
       </c>
@@ -12747,7 +12747,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>670</v>
       </c>
@@ -12815,7 +12815,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>307</v>
       </c>
@@ -12883,7 +12883,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="133" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>313</v>
       </c>
@@ -12951,7 +12951,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>307</v>
       </c>
@@ -13019,7 +13019,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="135" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>138</v>
       </c>
@@ -13087,7 +13087,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>307</v>
       </c>
@@ -13155,7 +13155,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>399</v>
       </c>
@@ -13223,7 +13223,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="138" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>304</v>
       </c>
@@ -13291,7 +13291,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="139" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>647</v>
       </c>
@@ -13359,7 +13359,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="140" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>596</v>
       </c>
@@ -13427,7 +13427,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="141" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>596</v>
       </c>
@@ -13495,7 +13495,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="142" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>444</v>
       </c>
@@ -13563,7 +13563,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="143" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>61</v>
       </c>
@@ -13631,7 +13631,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="144" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>61</v>
       </c>
@@ -13699,7 +13699,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="145" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>61</v>
       </c>
@@ -13767,7 +13767,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="146" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>61</v>
       </c>
@@ -13835,7 +13835,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="147" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>61</v>
       </c>
@@ -13903,7 +13903,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="148" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>61</v>
       </c>
@@ -13971,7 +13971,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="149" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>61</v>
       </c>
@@ -14039,7 +14039,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="150" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>61</v>
       </c>
@@ -14107,7 +14107,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="151" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>100</v>
       </c>
@@ -14175,7 +14175,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="152" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>733</v>
       </c>
@@ -14243,7 +14243,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="153" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>792</v>
       </c>
@@ -14311,7 +14311,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="154" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>776</v>
       </c>
@@ -14379,7 +14379,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="155" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>163</v>
       </c>
@@ -14447,7 +14447,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="156" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>867</v>
       </c>
@@ -14515,7 +14515,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="157" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>46</v>
       </c>
@@ -14583,7 +14583,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="158" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>46</v>
       </c>
@@ -14651,7 +14651,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="159" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>46</v>
       </c>
@@ -14719,7 +14719,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="160" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>46</v>
       </c>
@@ -14787,7 +14787,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="161" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>46</v>
       </c>
@@ -14855,7 +14855,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="162" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>46</v>
       </c>
@@ -14923,7 +14923,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="163" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>46</v>
       </c>
@@ -14991,7 +14991,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="164" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>46</v>
       </c>
@@ -15059,7 +15059,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="165" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>46</v>
       </c>
@@ -15127,7 +15127,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="166" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>46</v>
       </c>
@@ -15195,7 +15195,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="167" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>46</v>
       </c>
@@ -15263,7 +15263,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="168" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>46</v>
       </c>
@@ -15331,7 +15331,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="169" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>249</v>
       </c>
@@ -15399,7 +15399,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="170" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>249</v>
       </c>
@@ -15467,7 +15467,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="171" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>184</v>
       </c>
@@ -15535,7 +15535,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="172" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>249</v>
       </c>
@@ -15603,7 +15603,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="173" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>184</v>
       </c>
@@ -15671,7 +15671,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="174" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>389</v>
       </c>
@@ -15739,7 +15739,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="175" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>404</v>
       </c>
@@ -15807,7 +15807,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="176" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>71</v>
       </c>
@@ -15875,7 +15875,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="177" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>71</v>
       </c>
@@ -15943,7 +15943,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="178" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>71</v>
       </c>
@@ -16011,7 +16011,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="179" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>71</v>
       </c>
@@ -16079,7 +16079,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="180" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>71</v>
       </c>
@@ -16147,7 +16147,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="181" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>350</v>
       </c>
@@ -16215,7 +16215,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="182" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>350</v>
       </c>
@@ -16283,7 +16283,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="183" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>217</v>
       </c>
@@ -16351,7 +16351,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="184" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>220</v>
       </c>
@@ -16419,7 +16419,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="185" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>120</v>
       </c>
@@ -16487,7 +16487,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="186" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>91</v>
       </c>
@@ -16555,7 +16555,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="187" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>91</v>
       </c>
@@ -16623,7 +16623,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="188" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>120</v>
       </c>
@@ -16691,7 +16691,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="189" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>765</v>
       </c>
@@ -16759,7 +16759,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="190" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>256</v>
       </c>
@@ -16827,7 +16827,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="191" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>163</v>
       </c>
@@ -16895,7 +16895,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="192" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>163</v>
       </c>
@@ -16963,7 +16963,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="193" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>163</v>
       </c>
@@ -17031,7 +17031,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="194" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>194</v>
       </c>
@@ -17099,7 +17099,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="195" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>679</v>
       </c>
@@ -17167,7 +17167,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="196" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>194</v>
       </c>
@@ -17235,7 +17235,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="197" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>468</v>
       </c>
@@ -17303,7 +17303,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="198" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>368</v>
       </c>
@@ -17371,7 +17371,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="199" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>502</v>
       </c>
@@ -17439,7 +17439,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="200" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>168</v>
       </c>
@@ -17507,7 +17507,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="201" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>168</v>
       </c>
@@ -17575,7 +17575,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="202" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>237</v>
       </c>
@@ -17643,7 +17643,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="203" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>237</v>
       </c>
@@ -17711,7 +17711,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="204" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>566</v>
       </c>
@@ -17779,7 +17779,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="205" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>569</v>
       </c>
@@ -17847,7 +17847,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="206" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>601</v>
       </c>
@@ -17915,7 +17915,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="207" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>194</v>
       </c>
@@ -17983,7 +17983,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="208" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>194</v>
       </c>
@@ -18051,7 +18051,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="209" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>495</v>
       </c>
@@ -18119,7 +18119,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="210" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>350</v>
       </c>
@@ -18187,7 +18187,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="211" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>194</v>
       </c>
@@ -18255,7 +18255,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="212" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>870</v>
       </c>
@@ -18323,7 +18323,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="213" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>271</v>
       </c>
@@ -18391,7 +18391,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="214" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>271</v>
       </c>
@@ -18459,7 +18459,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="215" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>267</v>
       </c>
@@ -18527,7 +18527,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="216" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>414</v>
       </c>
@@ -18595,7 +18595,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="217" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>414</v>
       </c>
@@ -18663,7 +18663,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="218" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>874</v>
       </c>
@@ -18731,7 +18731,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="219" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>138</v>
       </c>
@@ -18799,7 +18799,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="220" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>138</v>
       </c>
@@ -18867,7 +18867,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="221" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>265</v>
       </c>
@@ -18935,7 +18935,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="222" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>773</v>
       </c>
@@ -19003,7 +19003,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="223" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>86</v>
       </c>
@@ -19071,7 +19071,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="224" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>86</v>
       </c>
@@ -19139,7 +19139,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="225" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>86</v>
       </c>
@@ -19207,7 +19207,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="226" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>539</v>
       </c>
@@ -19275,7 +19275,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="227" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>86</v>
       </c>
@@ -19343,7 +19343,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="228" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>86</v>
       </c>
@@ -19411,7 +19411,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="229" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>510</v>
       </c>
@@ -19479,7 +19479,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="230" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>271</v>
       </c>
@@ -19547,7 +19547,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="231" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>103</v>
       </c>
@@ -19615,7 +19615,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="232" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>228</v>
       </c>
@@ -19683,7 +19683,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="233" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>232</v>
       </c>
@@ -19751,7 +19751,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="234" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>49</v>
       </c>
@@ -19819,7 +19819,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="235" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>171</v>
       </c>
@@ -19887,7 +19887,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="236" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>171</v>
       </c>
@@ -19955,7 +19955,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="237" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>171</v>
       </c>
@@ -20023,7 +20023,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="238" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>49</v>
       </c>
@@ -20091,7 +20091,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="239" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>792</v>
       </c>
@@ -20159,7 +20159,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="240" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>66</v>
       </c>
@@ -20227,7 +20227,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="241" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>66</v>
       </c>
@@ -20295,7 +20295,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="242" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>66</v>
       </c>
@@ -20363,7 +20363,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="243" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>66</v>
       </c>
@@ -20431,7 +20431,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="244" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>66</v>
       </c>
@@ -20499,7 +20499,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="245" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>66</v>
       </c>
@@ -20567,7 +20567,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="246" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>66</v>
       </c>
@@ -20635,7 +20635,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="247" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
         <v>241</v>
       </c>
@@ -20703,7 +20703,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="248" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>49</v>
       </c>
@@ -20771,7 +20771,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="249" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
         <v>537</v>
       </c>
@@ -20839,7 +20839,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="250" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>241</v>
       </c>
@@ -20907,7 +20907,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="251" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
         <v>40</v>
       </c>
@@ -20975,7 +20975,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="252" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>40</v>
       </c>
@@ -21043,7 +21043,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="253" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>191</v>
       </c>
@@ -21111,7 +21111,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="254" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
         <v>193</v>
       </c>
@@ -21179,7 +21179,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="255" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>191</v>
       </c>
@@ -21247,7 +21247,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="256" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>38</v>
       </c>
@@ -21315,7 +21315,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="257" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
         <v>191</v>
       </c>
@@ -21383,7 +21383,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="258" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
         <v>812</v>
       </c>
@@ -21451,7 +21451,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="259" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
         <v>66</v>
       </c>
@@ -21519,7 +21519,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="260" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
         <v>179</v>
       </c>
@@ -21587,7 +21587,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="261" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
         <v>66</v>
       </c>
@@ -21655,7 +21655,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="262" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
         <v>179</v>
       </c>
@@ -21723,7 +21723,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="263" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
         <v>66</v>
       </c>
@@ -21791,7 +21791,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="264" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
         <v>563</v>
       </c>
@@ -21859,7 +21859,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="265" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
         <v>592</v>
       </c>
@@ -21927,7 +21927,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="266" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A266" s="1" t="s">
         <v>663</v>
       </c>
@@ -21995,7 +21995,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="267" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A267" s="1" t="s">
         <v>668</v>
       </c>
@@ -22063,7 +22063,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="268" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
         <v>688</v>
       </c>
@@ -22131,7 +22131,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="269" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
         <v>688</v>
       </c>
@@ -22199,7 +22199,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="270" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A270" s="1" t="s">
         <v>688</v>
       </c>
@@ -22267,7 +22267,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="271" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A271" s="1" t="s">
         <v>20</v>
       </c>
@@ -22335,7 +22335,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="272" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A272" s="1" t="s">
         <v>58</v>
       </c>
@@ -22403,7 +22403,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="273" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A273" s="1" t="s">
         <v>58</v>
       </c>
@@ -22471,7 +22471,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="274" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A274" s="1" t="s">
         <v>58</v>
       </c>
@@ -22539,7 +22539,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="275" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A275" s="1" t="s">
         <v>58</v>
       </c>
@@ -22607,7 +22607,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="276" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A276" s="1" t="s">
         <v>20</v>
       </c>
@@ -22675,7 +22675,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="277" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A277" s="1" t="s">
         <v>58</v>
       </c>
@@ -22743,7 +22743,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="278" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A278" s="1" t="s">
         <v>58</v>
       </c>
@@ -22811,7 +22811,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="279" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A279" s="1" t="s">
         <v>33</v>
       </c>
@@ -22879,7 +22879,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="280" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A280" s="1" t="s">
         <v>82</v>
       </c>
@@ -22947,7 +22947,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="281" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A281" s="1" t="s">
         <v>297</v>
       </c>
@@ -23015,7 +23015,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="282" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A282" s="1" t="s">
         <v>126</v>
       </c>
@@ -23083,7 +23083,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="283" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A283" s="1" t="s">
         <v>82</v>
       </c>
@@ -23151,7 +23151,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="284" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A284" s="1" t="s">
         <v>126</v>
       </c>
@@ -23219,7 +23219,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="285" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A285" s="1" t="s">
         <v>82</v>
       </c>
@@ -23287,7 +23287,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="286" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A286" s="1" t="s">
         <v>320</v>
       </c>
@@ -23355,7 +23355,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="287" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A287" s="1" t="s">
         <v>33</v>
       </c>
@@ -23423,7 +23423,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="288" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A288" s="1" t="s">
         <v>33</v>
       </c>
@@ -23491,7 +23491,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="289" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A289" s="1" t="s">
         <v>33</v>
       </c>
@@ -23559,7 +23559,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="290" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A290" s="1" t="s">
         <v>733</v>
       </c>
@@ -23627,7 +23627,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="291" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A291" s="1" t="s">
         <v>571</v>
       </c>
@@ -23695,7 +23695,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="292" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A292" s="1" t="s">
         <v>252</v>
       </c>
@@ -23763,7 +23763,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="293" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A293" s="1" t="s">
         <v>295</v>
       </c>
@@ -23831,7 +23831,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="294" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A294" s="1" t="s">
         <v>603</v>
       </c>
@@ -23899,7 +23899,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="295" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A295" s="1" t="s">
         <v>317</v>
       </c>
@@ -23967,7 +23967,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="296" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A296" s="1" t="s">
         <v>147</v>
       </c>
@@ -24035,7 +24035,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="297" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A297" s="1" t="s">
         <v>617</v>
       </c>
@@ -24103,7 +24103,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="298" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A298" s="1" t="s">
         <v>860</v>
       </c>
@@ -24171,7 +24171,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="299" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A299" s="1" t="s">
         <v>147</v>
       </c>
@@ -24239,7 +24239,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="300" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A300" s="1" t="s">
         <v>141</v>
       </c>
@@ -24307,7 +24307,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="301" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A301" s="1" t="s">
         <v>267</v>
       </c>
@@ -24375,7 +24375,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="302" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A302" s="1" t="s">
         <v>397</v>
       </c>
@@ -24443,7 +24443,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="303" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A303" s="1" t="s">
         <v>150</v>
       </c>
@@ -24511,7 +24511,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="304" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A304" s="1" t="s">
         <v>649</v>
       </c>
@@ -24579,7 +24579,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="305" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A305" s="1" t="s">
         <v>617</v>
       </c>
@@ -24647,7 +24647,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="306" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A306" s="1" t="s">
         <v>884</v>
       </c>
@@ -24715,7 +24715,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="307" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A307" s="1" t="s">
         <v>317</v>
       </c>
@@ -24783,7 +24783,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="308" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A308" s="1" t="s">
         <v>887</v>
       </c>
@@ -24851,7 +24851,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="309" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A309" s="1" t="s">
         <v>921</v>
       </c>
@@ -24919,7 +24919,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="310" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A310" s="1" t="s">
         <v>420</v>
       </c>
@@ -24987,7 +24987,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="311" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A311" s="1" t="s">
         <v>730</v>
       </c>
@@ -25055,7 +25055,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="312" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A312" s="1" t="s">
         <v>420</v>
       </c>
@@ -25123,7 +25123,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="313" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A313" s="1" t="s">
         <v>420</v>
       </c>
@@ -25191,7 +25191,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="314" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A314" s="1" t="s">
         <v>66</v>
       </c>
@@ -25259,7 +25259,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="315" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A315" s="1" t="s">
         <v>66</v>
       </c>
@@ -25327,7 +25327,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="316" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A316" s="1" t="s">
         <v>66</v>
       </c>
@@ -25395,7 +25395,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="317" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A317" s="1" t="s">
         <v>66</v>
       </c>
@@ -25463,7 +25463,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="318" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A318" s="1" t="s">
         <v>802</v>
       </c>
@@ -25531,7 +25531,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="319" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A319" s="1" t="s">
         <v>109</v>
       </c>
@@ -25599,7 +25599,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="320" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A320" s="1" t="s">
         <v>256</v>
       </c>
@@ -25667,7 +25667,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="321" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A321" s="1" t="s">
         <v>736</v>
       </c>
@@ -25735,7 +25735,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="322" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A322" s="1" t="s">
         <v>744</v>
       </c>
@@ -25803,7 +25803,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="323" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A323" s="1" t="s">
         <v>88</v>
       </c>
@@ -25871,7 +25871,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="324" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A324" s="1" t="s">
         <v>88</v>
       </c>
@@ -25939,7 +25939,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="325" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A325" s="1" t="s">
         <v>88</v>
       </c>
@@ -26007,7 +26007,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="326" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A326" s="1" t="s">
         <v>88</v>
       </c>
@@ -26075,7 +26075,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="327" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A327" s="1" t="s">
         <v>150</v>
       </c>
@@ -26143,7 +26143,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="328" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A328" s="1" t="s">
         <v>647</v>
       </c>
@@ -26211,7 +26211,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="329" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A329" s="1" t="s">
         <v>286</v>
       </c>
@@ -26279,7 +26279,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="330" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A330" s="1" t="s">
         <v>292</v>
       </c>
@@ -26347,7 +26347,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="331" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A331" s="1" t="s">
         <v>292</v>
       </c>
@@ -26415,7 +26415,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="332" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A332" s="1" t="s">
         <v>292</v>
       </c>
@@ -26483,7 +26483,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="333" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A333" s="1" t="s">
         <v>20</v>
       </c>
@@ -26551,7 +26551,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="334" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A334" s="1" t="s">
         <v>690</v>
       </c>
@@ -26619,7 +26619,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="335" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A335" s="1" t="s">
         <v>720</v>
       </c>
@@ -26687,7 +26687,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="336" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A336" s="1" t="s">
         <v>113</v>
       </c>
@@ -26755,7 +26755,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="337" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A337" s="1" t="s">
         <v>184</v>
       </c>
@@ -26823,7 +26823,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="338" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A338" s="1" t="s">
         <v>249</v>
       </c>
@@ -26891,7 +26891,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="339" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A339" s="1" t="s">
         <v>249</v>
       </c>
@@ -26959,7 +26959,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="340" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A340" s="1" t="s">
         <v>355</v>
       </c>
@@ -27027,7 +27027,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="341" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A341" s="1" t="s">
         <v>82</v>
       </c>
@@ -27095,7 +27095,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="342" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A342" s="1" t="s">
         <v>355</v>
       </c>
@@ -27163,7 +27163,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="343" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A343" s="1" t="s">
         <v>82</v>
       </c>
@@ -27231,7 +27231,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="344" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A344" s="1" t="s">
         <v>126</v>
       </c>
@@ -27299,7 +27299,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="345" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A345" s="1" t="s">
         <v>297</v>
       </c>
@@ -27367,7 +27367,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="346" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A346" s="1" t="s">
         <v>355</v>
       </c>
@@ -27435,7 +27435,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="347" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A347" s="1" t="s">
         <v>355</v>
       </c>
@@ -27503,7 +27503,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="348" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A348" s="1" t="s">
         <v>350</v>
       </c>
@@ -27571,7 +27571,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="349" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A349" s="1" t="s">
         <v>355</v>
       </c>
@@ -27639,7 +27639,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="350" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A350" s="1" t="s">
         <v>350</v>
       </c>
@@ -27707,7 +27707,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="351" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A351" s="1" t="s">
         <v>297</v>
       </c>
@@ -27775,7 +27775,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="352" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A352" s="1" t="s">
         <v>297</v>
       </c>
@@ -27843,7 +27843,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="353" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A353" s="1" t="s">
         <v>210</v>
       </c>
@@ -27911,7 +27911,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="354" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A354" s="1" t="s">
         <v>210</v>
       </c>
@@ -27979,7 +27979,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="355" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A355" s="1" t="s">
         <v>179</v>
       </c>
@@ -28047,7 +28047,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="356" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A356" s="1" t="s">
         <v>179</v>
       </c>
@@ -28115,7 +28115,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="357" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A357" s="1" t="s">
         <v>179</v>
       </c>
@@ -28183,7 +28183,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="358" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A358" s="1" t="s">
         <v>179</v>
       </c>
@@ -28251,7 +28251,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="359" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A359" s="1" t="s">
         <v>58</v>
       </c>
@@ -28319,7 +28319,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="360" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A360" s="1" t="s">
         <v>20</v>
       </c>
@@ -28387,7 +28387,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="361" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A361" s="1" t="s">
         <v>20</v>
       </c>
@@ -28455,7 +28455,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="362" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A362" s="1" t="s">
         <v>20</v>
       </c>
@@ -28523,7 +28523,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="363" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A363" s="1" t="s">
         <v>249</v>
       </c>
@@ -28591,7 +28591,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="364" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A364" s="1" t="s">
         <v>184</v>
       </c>
@@ -28659,7 +28659,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="365" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A365" s="1" t="s">
         <v>113</v>
       </c>
@@ -28727,7 +28727,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="366" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A366" s="1" t="s">
         <v>249</v>
       </c>
@@ -28795,7 +28795,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="367" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A367" s="1" t="s">
         <v>168</v>
       </c>
@@ -28863,7 +28863,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="368" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A368" s="1" t="s">
         <v>372</v>
       </c>
@@ -28931,7 +28931,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="369" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A369" s="1" t="s">
         <v>372</v>
       </c>
@@ -28999,7 +28999,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="370" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A370" s="1" t="s">
         <v>168</v>
       </c>
@@ -29067,7 +29067,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="371" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A371" s="1" t="s">
         <v>372</v>
       </c>
@@ -29135,7 +29135,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="372" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A372" s="1" t="s">
         <v>815</v>
       </c>
@@ -29203,7 +29203,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="373" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A373" s="1" t="s">
         <v>126</v>
       </c>
@@ -29271,7 +29271,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="374" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A374" s="1" t="s">
         <v>193</v>
       </c>
@@ -29339,7 +29339,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="375" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A375" s="1" t="s">
         <v>297</v>
       </c>
@@ -29407,7 +29407,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="376" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A376" s="1" t="s">
         <v>176</v>
       </c>
@@ -29475,7 +29475,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="377" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A377" s="1" t="s">
         <v>176</v>
       </c>
@@ -29543,7 +29543,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="378" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A378" s="1" t="s">
         <v>40</v>
       </c>
@@ -29611,7 +29611,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="379" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A379" s="1" t="s">
         <v>91</v>
       </c>
@@ -29679,7 +29679,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="380" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A380" s="1" t="s">
         <v>173</v>
       </c>
@@ -29747,7 +29747,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="381" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A381" s="1" t="s">
         <v>173</v>
       </c>
@@ -29815,7 +29815,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="382" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A382" s="1" t="s">
         <v>173</v>
       </c>
@@ -29883,7 +29883,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="383" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A383" s="1" t="s">
         <v>256</v>
       </c>
@@ -29951,7 +29951,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="384" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A384" s="1" t="s">
         <v>163</v>
       </c>
@@ -30019,7 +30019,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="385" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A385" s="1" t="s">
         <v>163</v>
       </c>
@@ -30087,7 +30087,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="386" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A386" s="1" t="s">
         <v>406</v>
       </c>
@@ -30155,7 +30155,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="387" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A387" s="1" t="s">
         <v>406</v>
       </c>
@@ -30223,7 +30223,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="388" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A388" s="1" t="s">
         <v>328</v>
       </c>
@@ -30291,7 +30291,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="389" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A389" s="1" t="s">
         <v>153</v>
       </c>
@@ -30359,7 +30359,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="390" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A390" s="1" t="s">
         <v>600</v>
       </c>
@@ -30427,7 +30427,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="391" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A391" s="1" t="s">
         <v>749</v>
       </c>
@@ -30495,7 +30495,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="392" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A392" s="1" t="s">
         <v>749</v>
       </c>
@@ -30563,7 +30563,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="393" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A393" s="1" t="s">
         <v>897</v>
       </c>
@@ -30631,7 +30631,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="394" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A394" s="1" t="s">
         <v>40</v>
       </c>
@@ -30699,7 +30699,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="395" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A395" s="1" t="s">
         <v>241</v>
       </c>
@@ -30767,7 +30767,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="396" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A396" s="1" t="s">
         <v>241</v>
       </c>
@@ -30835,7 +30835,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="397" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A397" s="1" t="s">
         <v>241</v>
       </c>
@@ -30903,7 +30903,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="398" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A398" s="1" t="s">
         <v>40</v>
       </c>
@@ -30971,7 +30971,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="399" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A399" s="1" t="s">
         <v>82</v>
       </c>
@@ -31039,7 +31039,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="400" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A400" s="1" t="s">
         <v>176</v>
       </c>
@@ -31107,7 +31107,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="401" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A401" s="1" t="s">
         <v>191</v>
       </c>
@@ -31175,7 +31175,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="402" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A402" s="1" t="s">
         <v>193</v>
       </c>
@@ -31243,7 +31243,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="403" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A403" s="1" t="s">
         <v>193</v>
       </c>
@@ -31311,7 +31311,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="404" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A404" s="1" t="s">
         <v>193</v>
       </c>
@@ -31379,7 +31379,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="405" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A405" s="1" t="s">
         <v>193</v>
       </c>
@@ -31447,7 +31447,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="406" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A406" s="1" t="s">
         <v>176</v>
       </c>
@@ -31515,7 +31515,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="407" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A407" s="1" t="s">
         <v>38</v>
       </c>
@@ -31583,7 +31583,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="408" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A408" s="1" t="s">
         <v>753</v>
       </c>
@@ -31651,7 +31651,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="409" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A409" s="1" t="s">
         <v>220</v>
       </c>
@@ -31719,7 +31719,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="410" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A410" s="1" t="s">
         <v>58</v>
       </c>
@@ -31787,7 +31787,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="411" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A411" s="1" t="s">
         <v>20</v>
       </c>
@@ -31855,7 +31855,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="412" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A412" s="1" t="s">
         <v>58</v>
       </c>
@@ -31923,7 +31923,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="413" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A413" s="1" t="s">
         <v>20</v>
       </c>
@@ -31991,7 +31991,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="414" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A414" s="1" t="s">
         <v>20</v>
       </c>
@@ -32059,7 +32059,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="415" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A415" s="1" t="s">
         <v>20</v>
       </c>
@@ -32127,7 +32127,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="416" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A416" s="1" t="s">
         <v>20</v>
       </c>
@@ -32195,7 +32195,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="417" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A417" s="1" t="s">
         <v>314</v>
       </c>
@@ -32263,7 +32263,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="418" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A418" s="1" t="s">
         <v>404</v>
       </c>
@@ -32331,7 +32331,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="419" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A419" s="1" t="s">
         <v>210</v>
       </c>
@@ -32399,7 +32399,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="420" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A420" s="1" t="s">
         <v>399</v>
       </c>
@@ -32467,7 +32467,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="421" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A421" s="1" t="s">
         <v>852</v>
       </c>
@@ -32535,7 +32535,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="422" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A422" s="1" t="s">
         <v>700</v>
       </c>
@@ -32603,7 +32603,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="423" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A423" s="1" t="s">
         <v>304</v>
       </c>
@@ -32671,7 +32671,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="424" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A424" s="1" t="s">
         <v>38</v>
       </c>
@@ -32739,7 +32739,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="425" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A425" s="1" t="s">
         <v>193</v>
       </c>
@@ -32807,7 +32807,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="426" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A426" s="1" t="s">
         <v>191</v>
       </c>
@@ -32875,7 +32875,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="427" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A427" s="1" t="s">
         <v>191</v>
       </c>
@@ -32943,7 +32943,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="428" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A428" s="1" t="s">
         <v>43</v>
       </c>
@@ -33011,7 +33011,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="429" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A429" s="1" t="s">
         <v>43</v>
       </c>
@@ -33079,7 +33079,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="430" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A430" s="1" t="s">
         <v>43</v>
       </c>
@@ -33147,7 +33147,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="431" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A431" s="1" t="s">
         <v>43</v>
       </c>
@@ -33215,7 +33215,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="432" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A432" s="1" t="s">
         <v>43</v>
       </c>
@@ -33283,7 +33283,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="433" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A433" s="1" t="s">
         <v>43</v>
       </c>
@@ -33351,7 +33351,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="434" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A434" s="1" t="s">
         <v>113</v>
       </c>
@@ -33419,7 +33419,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="435" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A435" s="1" t="s">
         <v>120</v>
       </c>
@@ -33487,7 +33487,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="436" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A436" s="1" t="s">
         <v>113</v>
       </c>
@@ -33555,7 +33555,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="437" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A437" s="1" t="s">
         <v>292</v>
       </c>
@@ -33623,7 +33623,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="438" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A438" s="1" t="s">
         <v>579</v>
       </c>
@@ -33691,7 +33691,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="439" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A439" s="1" t="s">
         <v>113</v>
       </c>
@@ -33759,7 +33759,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="440" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A440" s="1" t="s">
         <v>292</v>
       </c>
@@ -33827,7 +33827,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="441" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A441" s="1" t="s">
         <v>256</v>
       </c>
@@ -33895,7 +33895,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="442" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A442" s="1" t="s">
         <v>736</v>
       </c>
@@ -33963,7 +33963,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="443" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A443" s="1" t="s">
         <v>717</v>
       </c>
@@ -34031,7 +34031,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="444" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A444" s="1" t="s">
         <v>909</v>
       </c>
@@ -34099,7 +34099,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="445" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A445" s="1" t="s">
         <v>818</v>
       </c>
@@ -34167,7 +34167,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="446" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A446" s="1" t="s">
         <v>234</v>
       </c>
@@ -34235,7 +34235,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="447" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A447" s="1" t="s">
         <v>144</v>
       </c>
@@ -34303,7 +34303,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="448" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A448" s="1" t="s">
         <v>150</v>
       </c>
@@ -34371,7 +34371,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="449" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A449" s="1" t="s">
         <v>476</v>
       </c>
@@ -34439,7 +34439,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="450" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A450" s="1" t="s">
         <v>614</v>
       </c>
@@ -34507,7 +34507,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="451" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A451" s="1" t="s">
         <v>150</v>
       </c>
@@ -34575,7 +34575,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="452" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A452" s="1" t="s">
         <v>585</v>
       </c>
@@ -34643,7 +34643,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="453" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A453" s="1" t="s">
         <v>594</v>
       </c>
@@ -34711,7 +34711,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="454" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A454" s="1" t="s">
         <v>94</v>
       </c>
@@ -34779,7 +34779,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="455" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A455" s="1" t="s">
         <v>763</v>
       </c>
@@ -34847,7 +34847,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="456" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A456" s="1" t="s">
         <v>173</v>
       </c>
@@ -34915,7 +34915,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="457" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A457" s="1" t="s">
         <v>173</v>
       </c>
@@ -34983,7 +34983,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="458" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A458" s="1" t="s">
         <v>91</v>
       </c>
@@ -35051,7 +35051,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="459" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A459" s="1" t="s">
         <v>91</v>
       </c>
@@ -35119,7 +35119,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="460" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A460" s="1" t="s">
         <v>485</v>
       </c>
@@ -35187,7 +35187,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="461" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A461" s="1" t="s">
         <v>173</v>
       </c>
@@ -35255,7 +35255,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="462" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A462" s="1" t="s">
         <v>173</v>
       </c>
@@ -35323,7 +35323,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="463" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A463" s="1" t="s">
         <v>91</v>
       </c>
@@ -35391,7 +35391,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="464" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A464" s="1" t="s">
         <v>123</v>
       </c>
@@ -35459,7 +35459,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="465" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A465" s="1" t="s">
         <v>91</v>
       </c>
@@ -35527,7 +35527,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="466" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A466" s="1" t="s">
         <v>861</v>
       </c>
@@ -35595,7 +35595,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="467" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A467" s="1" t="s">
         <v>460</v>
       </c>
@@ -35663,7 +35663,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="468" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A468" s="1" t="s">
         <v>460</v>
       </c>
@@ -35731,7 +35731,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="469" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A469" s="1" t="s">
         <v>38</v>
       </c>
@@ -35799,7 +35799,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="470" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A470" s="1" t="s">
         <v>86</v>
       </c>
@@ -35867,7 +35867,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="471" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A471" s="1" t="s">
         <v>193</v>
       </c>
@@ -35935,7 +35935,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="472" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A472" s="1" t="s">
         <v>193</v>
       </c>
@@ -36003,7 +36003,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="473" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A473" s="1" t="s">
         <v>193</v>
       </c>
@@ -36071,7 +36071,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="474" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A474" s="1" t="s">
         <v>906</v>
       </c>
@@ -36139,7 +36139,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="475" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A475" s="1" t="s">
         <v>436</v>
       </c>
@@ -36207,7 +36207,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="476" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A476" s="1" t="s">
         <v>439</v>
       </c>
@@ -36275,7 +36275,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="477" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A477" s="1" t="s">
         <v>265</v>
       </c>
@@ -36343,7 +36343,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="478" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A478" s="1" t="s">
         <v>163</v>
       </c>
@@ -36411,7 +36411,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="479" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A479" s="1" t="s">
         <v>163</v>
       </c>
@@ -36479,7 +36479,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="480" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A480" s="1" t="s">
         <v>106</v>
       </c>
@@ -36547,7 +36547,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="481" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A481" s="1" t="s">
         <v>201</v>
       </c>
@@ -36615,7 +36615,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="482" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A482" s="1" t="s">
         <v>201</v>
       </c>
@@ -36683,7 +36683,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="483" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A483" s="1" t="s">
         <v>217</v>
       </c>
@@ -36751,7 +36751,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="484" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A484" s="1" t="s">
         <v>444</v>
       </c>
@@ -36819,7 +36819,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="485" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A485" s="1" t="s">
         <v>444</v>
       </c>
@@ -36887,7 +36887,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="486" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A486" s="1" t="s">
         <v>596</v>
       </c>
@@ -36955,7 +36955,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="487" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A487" s="1" t="s">
         <v>444</v>
       </c>
@@ -37023,7 +37023,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="488" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A488" s="1" t="s">
         <v>82</v>
       </c>
@@ -37091,7 +37091,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="489" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A489" s="1" t="s">
         <v>374</v>
       </c>
@@ -37159,7 +37159,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="490" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A490" s="1" t="s">
         <v>188</v>
       </c>
@@ -37227,7 +37227,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="491" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A491" s="1" t="s">
         <v>38</v>
       </c>
@@ -37295,7 +37295,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="492" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A492" s="1" t="s">
         <v>184</v>
       </c>
@@ -37363,7 +37363,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="493" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A493" s="1" t="s">
         <v>193</v>
       </c>
@@ -37432,8 +37432,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V493" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:V1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter>
     <oddHeader>Danh sách nhóm tổ mô hình TKB ngày: đã nhập công thức học</oddHeader>
     <evenFooter>Danh sách nhóm tổ mô hình TKB ngày: đã nhập công thức học</evenFooter>

</xml_diff>